<commit_message>
Read from files to excel (done)
</commit_message>
<xml_diff>
--- a/Chapter_12/1.xlsx
+++ b/Chapter_12/1.xlsx
@@ -1,32 +1,108 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+  <si>
+    <t xml:space="preserve">Dong 1 file 1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dong 1 file 2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dong 1 file 3
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dong 2 file 1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dong 2 file 2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dong 2 file 3
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dong 3 file 1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dong 3 file 2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dong 3 file 3
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dong 4 file 1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dong 4 file 2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dong 4 file 3
+</t>
+  </si>
+  <si>
+    <t>Dong 5 file 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dong 5 file 2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dong 5 file 3
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dong 6 file 2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dong 6 file 3
+</t>
+  </si>
+  <si>
+    <t>Dong 7 file 2</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -42,21 +118,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -346,13 +416,88 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>